<commit_message>
added new features to script
</commit_message>
<xml_diff>
--- a/091322_PK_homologue code test.xlsx
+++ b/091322_PK_homologue code test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="204">
   <si>
     <t xml:space="preserve">Formula</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">Error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">delta m/z</t>
   </si>
   <si>
     <t xml:space="preserve">C214 H663 N243 O189</t>
@@ -880,10 +877,10 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.83"/>
@@ -905,13 +902,10 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>9661.97416</v>
@@ -926,13 +920,11 @@
         <f aca="false">5/(10^6)*C2</f>
         <v>0.0080566815</v>
       </c>
-      <c r="F2" s="7" t="n">
-        <v>71.037114</v>
-      </c>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>9626.98564</v>
@@ -950,7 +942,7 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>9555.98686</v>
@@ -968,7 +960,7 @@
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>9484.86064</v>
@@ -986,7 +978,7 @@
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>9271.80104</v>
@@ -1004,7 +996,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>8916.61434</v>
@@ -1022,7 +1014,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="n">
         <v>8845.59354</v>
@@ -1040,7 +1032,7 @@
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6" t="n">
         <v>8844.55912</v>
@@ -1058,7 +1050,7 @@
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="6" t="n">
         <v>8703.50399</v>
@@ -1076,7 +1068,7 @@
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="6" t="n">
         <v>8561.43762</v>
@@ -1094,7 +1086,7 @@
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="6" t="n">
         <v>8419.36092</v>
@@ -1112,7 +1104,7 @@
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="6" t="n">
         <v>8418.37162</v>
@@ -1130,7 +1122,7 @@
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" s="6" t="n">
         <v>8347.3459</v>
@@ -1148,7 +1140,7 @@
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="6" t="n">
         <v>8276.29863</v>
@@ -1166,7 +1158,7 @@
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" s="6" t="n">
         <v>8207.23962</v>
@@ -1184,7 +1176,7 @@
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="6" t="n">
         <v>8206.25346</v>
@@ -1202,7 +1194,7 @@
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="6" t="n">
         <v>8135.22245</v>
@@ -1220,7 +1212,7 @@
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="6" t="n">
         <v>8134.17363</v>
@@ -1238,7 +1230,7 @@
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="6" t="n">
         <v>8063.18353</v>
@@ -1256,7 +1248,7 @@
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" s="6" t="n">
         <v>7922.1029</v>
@@ -1274,7 +1266,7 @@
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="6" t="n">
         <v>7921.09338</v>
@@ -1292,7 +1284,7 @@
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="6" t="n">
         <v>7849.08955</v>
@@ -1310,7 +1302,7 @@
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="6" t="n">
         <v>7779.01826</v>
@@ -1328,7 +1320,7 @@
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="6" t="n">
         <v>7708.98047</v>
@@ -1346,7 +1338,7 @@
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" s="6" t="n">
         <v>7671.94116</v>
@@ -1364,7 +1356,7 @@
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="6" t="n">
         <v>7636.9436</v>
@@ -1382,7 +1374,7 @@
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" s="6" t="n">
         <v>7635.9591</v>
@@ -1400,7 +1392,7 @@
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="6" t="n">
         <v>7565.93656</v>
@@ -1418,7 +1410,7 @@
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="6" t="n">
         <v>7565.89807</v>
@@ -1436,7 +1428,7 @@
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="6" t="n">
         <v>7510.85961</v>
@@ -1454,7 +1446,7 @@
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="6" t="n">
         <v>7495.86877</v>
@@ -1472,7 +1464,7 @@
     </row>
     <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="6" t="n">
         <v>7494.90776</v>
@@ -1490,7 +1482,7 @@
     </row>
     <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="6" t="n">
         <v>7493.90405</v>
@@ -1508,7 +1500,7 @@
     </row>
     <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" s="6" t="n">
         <v>7423.84179</v>
@@ -1526,7 +1518,7 @@
     </row>
     <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="6" t="n">
         <v>7316.72814</v>
@@ -1544,7 +1536,7 @@
     </row>
     <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>7281.76599</v>
@@ -1562,7 +1554,7 @@
     </row>
     <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="6" t="n">
         <v>7210.73876</v>
@@ -1580,7 +1572,7 @@
     </row>
     <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="6" t="n">
         <v>7210.71374</v>
@@ -1598,7 +1590,7 @@
     </row>
     <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="6" t="n">
         <v>7138.71484</v>
@@ -1616,7 +1608,7 @@
     </row>
     <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" s="6" t="n">
         <v>7135.61669</v>
@@ -1634,7 +1626,7 @@
     </row>
     <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B42" s="6" t="n">
         <v>7084.63159</v>
@@ -1652,7 +1644,7 @@
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" s="6" t="n">
         <v>7068.66235</v>
@@ -1670,7 +1662,7 @@
     </row>
     <row r="44" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" s="6" t="n">
         <v>6996.6018</v>
@@ -1688,7 +1680,7 @@
     </row>
     <row r="45" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" s="6" t="n">
         <v>6961.54748</v>
@@ -1706,7 +1698,7 @@
     </row>
     <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" s="6" t="n">
         <v>6944.57726</v>
@@ -1724,7 +1716,7 @@
     </row>
     <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" s="6" t="n">
         <v>6943.56955</v>
@@ -1742,7 +1734,7 @@
     </row>
     <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" s="6" t="n">
         <v>6926.58105</v>
@@ -1760,7 +1752,7 @@
     </row>
     <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" s="6" t="n">
         <v>6925.56603</v>
@@ -1778,7 +1770,7 @@
     </row>
     <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="6" t="n">
         <v>6922.50573</v>
@@ -1796,7 +1788,7 @@
     </row>
     <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="6" t="n">
         <v>6851.4602</v>
@@ -1814,7 +1806,7 @@
     </row>
     <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" s="6" t="n">
         <v>6800.51415</v>
@@ -1832,7 +1824,7 @@
     </row>
     <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" s="6" t="n">
         <v>6783.51355</v>
@@ -1850,7 +1842,7 @@
     </row>
     <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" s="6" t="n">
         <v>6730.43359</v>
@@ -1868,7 +1860,7 @@
     </row>
     <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="6" t="n">
         <v>6728.45422</v>
@@ -1886,7 +1878,7 @@
     </row>
     <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="6" t="n">
         <v>6714.47228</v>
@@ -1904,7 +1896,7 @@
     </row>
     <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="6" t="n">
         <v>6712.47521</v>
@@ -1922,7 +1914,7 @@
     </row>
     <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" s="6" t="n">
         <v>6711.38452</v>
@@ -1940,7 +1932,7 @@
     </row>
     <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B59" s="6" t="n">
         <v>6710.40063</v>
@@ -1958,7 +1950,7 @@
     </row>
     <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" s="6" t="n">
         <v>6677.39221</v>
@@ -1976,7 +1968,7 @@
     </row>
     <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" s="6" t="n">
         <v>6675.39025</v>
@@ -1994,7 +1986,7 @@
     </row>
     <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="6" t="n">
         <v>6659.41125</v>
@@ -2012,7 +2004,7 @@
     </row>
     <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="6" t="n">
         <v>6658.40417</v>
@@ -2030,7 +2022,7 @@
     </row>
     <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" s="6" t="n">
         <v>6653.54577</v>
@@ -2048,7 +2040,7 @@
     </row>
     <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="6" t="n">
         <v>6641.42236</v>
@@ -2066,7 +2058,7 @@
     </row>
     <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="6" t="n">
         <v>6593.38952</v>
@@ -2084,7 +2076,7 @@
     </row>
     <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="6" t="n">
         <v>6587.3722</v>
@@ -2102,7 +2094,7 @@
     </row>
     <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" s="6" t="n">
         <v>6534.3496</v>
@@ -2120,7 +2112,7 @@
     </row>
     <row r="69" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" s="6" t="n">
         <v>6517.37084</v>
@@ -2138,7 +2130,7 @@
     </row>
     <row r="70" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" s="6" t="n">
         <v>6511.46996</v>
@@ -2156,7 +2148,7 @@
     </row>
     <row r="71" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" s="6" t="n">
         <v>6503.36847</v>
@@ -2174,7 +2166,7 @@
     </row>
     <row r="72" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" s="6" t="n">
         <v>6496.2787</v>
@@ -2192,7 +2184,7 @@
     </row>
     <row r="73" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" s="6" t="n">
         <v>6454.28857</v>
@@ -2210,7 +2202,7 @@
     </row>
     <row r="74" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" s="6" t="n">
         <v>6440.4287</v>
@@ -2228,7 +2220,7 @@
     </row>
     <row r="75" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75" s="6" t="n">
         <v>6430.32246</v>
@@ -2246,7 +2238,7 @@
     </row>
     <row r="76" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B76" s="6" t="n">
         <v>6429.33679</v>
@@ -2264,7 +2256,7 @@
     </row>
     <row r="77" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77" s="6" t="n">
         <v>6374.28927</v>
@@ -2282,7 +2274,7 @@
     </row>
     <row r="78" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" s="6" t="n">
         <v>6358.2821</v>
@@ -2300,7 +2292,7 @@
     </row>
     <row r="79" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B79" s="6" t="n">
         <v>6357.28159</v>
@@ -2318,7 +2310,7 @@
     </row>
     <row r="80" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B80" s="6" t="n">
         <v>6297.35659</v>
@@ -2336,7 +2328,7 @@
     </row>
     <row r="81" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B81" s="6" t="n">
         <v>6287.2498</v>
@@ -2354,7 +2346,7 @@
     </row>
     <row r="82" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" s="6" t="n">
         <v>6287.22431</v>
@@ -2372,7 +2364,7 @@
     </row>
     <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B83" s="6" t="n">
         <v>6233.20031</v>
@@ -2390,7 +2382,7 @@
     </row>
     <row r="84" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" s="6" t="n">
         <v>6231.18615</v>
@@ -2408,7 +2400,7 @@
     </row>
     <row r="85" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B85" s="6" t="n">
         <v>6217.19355</v>
@@ -2426,7 +2418,7 @@
     </row>
     <row r="86" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B86" s="6" t="n">
         <v>6216.21362</v>
@@ -2444,7 +2436,7 @@
     </row>
     <row r="87" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B87" s="6" t="n">
         <v>6215.16865</v>
@@ -2462,7 +2454,7 @@
     </row>
     <row r="88" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B88" s="6" t="n">
         <v>6212.10839</v>
@@ -2480,7 +2472,7 @@
     </row>
     <row r="89" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B89" s="6" t="n">
         <v>6177.14135</v>
@@ -2498,7 +2490,7 @@
     </row>
     <row r="90" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B90" s="6" t="n">
         <v>6177.12487</v>
@@ -2516,7 +2508,7 @@
     </row>
     <row r="91" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B91" s="6" t="n">
         <v>6161.16601</v>
@@ -2534,7 +2526,7 @@
     </row>
     <row r="92" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B92" s="6" t="n">
         <v>6145.17169</v>
@@ -2552,7 +2544,7 @@
     </row>
     <row r="93" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B93" s="6" t="n">
         <v>6144.16589</v>
@@ -2570,7 +2562,7 @@
     </row>
     <row r="94" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B94" s="6" t="n">
         <v>6107.08949</v>
@@ -2588,7 +2580,7 @@
     </row>
     <row r="95" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B95" s="6" t="n">
         <v>6090.12475</v>
@@ -2606,7 +2598,7 @@
     </row>
     <row r="96" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B96" s="6" t="n">
         <v>6084.24278</v>
@@ -2624,7 +2616,7 @@
     </row>
     <row r="97" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B97" s="6" t="n">
         <v>6074.13415</v>
@@ -2642,7 +2634,7 @@
     </row>
     <row r="98" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B98" s="6" t="n">
         <v>6036.05737</v>
@@ -2660,7 +2652,7 @@
     </row>
     <row r="99" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B99" s="6" t="n">
         <v>6035.01777</v>
@@ -2678,7 +2670,7 @@
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B100" s="6" t="n">
         <v>6033.09838</v>
@@ -2696,7 +2688,7 @@
     </row>
     <row r="101" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B101" s="6" t="n">
         <v>6026.0769</v>
@@ -2714,7 +2706,7 @@
     </row>
     <row r="102" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B102" s="6" t="n">
         <v>6019.09182</v>
@@ -2732,7 +2724,7 @@
     </row>
     <row r="103" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B103" s="6" t="n">
         <v>6019.07922</v>
@@ -2750,7 +2742,7 @@
     </row>
     <row r="104" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B104" s="6" t="n">
         <v>6003.08955</v>
@@ -2768,7 +2760,7 @@
     </row>
     <row r="105" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B105" s="6" t="n">
         <v>6002.10717</v>
@@ -2786,7 +2778,7 @@
     </row>
     <row r="106" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B106" s="6" t="n">
         <v>6002.07539</v>
@@ -2804,7 +2796,7 @@
     </row>
     <row r="107" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B107" s="6" t="n">
         <v>5965.01777</v>
@@ -2822,7 +2814,7 @@
     </row>
     <row r="108" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B108" s="6" t="n">
         <v>5956.04821</v>
@@ -2840,7 +2832,7 @@
     </row>
     <row r="109" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B109" s="6" t="n">
         <v>5942.17858</v>
@@ -2858,7 +2850,7 @@
     </row>
     <row r="110" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B110" s="6" t="n">
         <v>5932.05585</v>
@@ -2876,7 +2868,7 @@
     </row>
     <row r="111" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B111" s="6" t="n">
         <v>5931.06957</v>
@@ -2894,7 +2886,7 @@
     </row>
     <row r="112" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B112" s="6" t="n">
         <v>5931.03681</v>
@@ -2912,7 +2904,7 @@
     </row>
     <row r="113" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B113" s="6" t="n">
         <v>5896.00166</v>
@@ -2930,7 +2922,7 @@
     </row>
     <row r="114" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B114" s="6" t="n">
         <v>5876.01403</v>
@@ -2948,7 +2940,7 @@
     </row>
     <row r="115" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B115" s="6" t="n">
         <v>5871.12695</v>
@@ -2966,7 +2958,7 @@
     </row>
     <row r="116" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B116" s="6" t="n">
         <v>5861.0238</v>
@@ -2984,7 +2976,7 @@
     </row>
     <row r="117" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B117" s="6" t="n">
         <v>5860.01763</v>
@@ -3002,7 +2994,7 @@
     </row>
     <row r="118" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B118" s="6" t="n">
         <v>5816.95576</v>
@@ -3020,7 +3012,7 @@
     </row>
     <row r="119" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B119" s="6" t="n">
         <v>5800.08141</v>
@@ -3038,7 +3030,7 @@
     </row>
     <row r="120" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B120" s="6" t="n">
         <v>5788.97431</v>
@@ -3056,7 +3048,7 @@
     </row>
     <row r="121" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B121" s="6" t="n">
         <v>5750.90095</v>
@@ -3074,7 +3066,7 @@
     </row>
     <row r="122" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122" s="6" t="n">
         <v>5735.94746</v>
@@ -3092,7 +3084,7 @@
     </row>
     <row r="123" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B123" s="6" t="n">
         <v>5730.06371</v>
@@ -3110,7 +3102,7 @@
     </row>
     <row r="124" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B124" s="6" t="n">
         <v>5729.05724</v>
@@ -3128,7 +3120,7 @@
     </row>
     <row r="125" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B125" s="6" t="n">
         <v>5728.04528</v>
@@ -3146,7 +3138,7 @@
     </row>
     <row r="126" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B126" s="6" t="n">
         <v>5717.94064</v>
@@ -3164,7 +3156,7 @@
     </row>
     <row r="127" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B127" s="6" t="n">
         <v>5680.86933</v>
@@ -3182,7 +3174,7 @@
     </row>
     <row r="128" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B128" s="6" t="n">
         <v>5679.872</v>
@@ -3200,7 +3192,7 @@
     </row>
     <row r="129" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B129" s="6" t="n">
         <v>5678.83857</v>
@@ -3218,7 +3210,7 @@
     </row>
     <row r="130" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B130" s="6" t="n">
         <v>5646.90767</v>
@@ -3236,7 +3228,7 @@
     </row>
     <row r="131" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B131" s="6" t="n">
         <v>5646.8791</v>
@@ -3254,7 +3246,7 @@
     </row>
     <row r="132" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B132" s="6" t="n">
         <v>5600.84191</v>
@@ -3272,7 +3264,7 @@
     </row>
     <row r="133" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B133" s="6" t="n">
         <v>5599.87231</v>
@@ -3290,7 +3282,7 @@
     </row>
     <row r="134" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B134" s="6" t="n">
         <v>5592.85889</v>
@@ -3308,7 +3300,7 @@
     </row>
     <row r="135" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B135" s="6" t="n">
         <v>5586.98882</v>
@@ -3326,7 +3318,7 @@
     </row>
     <row r="136" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B136" s="6" t="n">
         <v>5576.8789</v>
@@ -3344,7 +3336,7 @@
     </row>
     <row r="137" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B137" s="6" t="n">
         <v>5575.89379</v>
@@ -3362,7 +3354,7 @@
     </row>
     <row r="138" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B138" s="6" t="n">
         <v>5575.87373</v>
@@ -3380,7 +3372,7 @@
     </row>
     <row r="139" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B139" s="6" t="n">
         <v>5521.82273</v>
@@ -3398,7 +3390,7 @@
     </row>
     <row r="140" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B140" s="6" t="n">
         <v>5508.8366</v>
@@ -3416,7 +3408,7 @@
     </row>
     <row r="141" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B141" s="6" t="n">
         <v>5504.82266</v>
@@ -3434,7 +3426,7 @@
     </row>
     <row r="142" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B142" s="6" t="n">
         <v>5501.73701</v>
@@ -3452,7 +3444,7 @@
     </row>
     <row r="143" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B143" s="6" t="n">
         <v>5488.86526</v>
@@ -3470,7 +3462,7 @@
     </row>
     <row r="144" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B144" s="6" t="n">
         <v>5466.75654</v>
@@ -3488,7 +3480,7 @@
     </row>
     <row r="145" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B145" s="6" t="n">
         <v>5465.7497</v>
@@ -3506,7 +3498,7 @@
     </row>
     <row r="146" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B146" s="6" t="n">
         <v>5450.79413</v>
@@ -3524,7 +3516,7 @@
     </row>
     <row r="147" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B147" s="6" t="n">
         <v>5449.7746</v>
@@ -3542,7 +3534,7 @@
     </row>
     <row r="148" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B148" s="6" t="n">
         <v>5444.91845</v>
@@ -3560,7 +3552,7 @@
     </row>
     <row r="149" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B149" s="6" t="n">
         <v>5434.79651</v>
@@ -3578,7 +3570,7 @@
     </row>
     <row r="150" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B150" s="6" t="n">
         <v>5430.71601</v>
@@ -3596,7 +3588,7 @@
     </row>
     <row r="151" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B151" s="6" t="n">
         <v>5395.7562</v>
@@ -3614,7 +3606,7 @@
     </row>
     <row r="152" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B152" s="6" t="n">
         <v>5395.72278</v>
@@ -3632,7 +3624,7 @@
     </row>
     <row r="153" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B153" s="6" t="n">
         <v>5379.75151</v>
@@ -3650,7 +3642,7 @@
     </row>
     <row r="154" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B154" s="6" t="n">
         <v>5363.76675</v>
@@ -3668,7 +3660,7 @@
     </row>
     <row r="155" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B155" s="6" t="n">
         <v>5362.76302</v>
@@ -3686,7 +3678,7 @@
     </row>
     <row r="156" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B156" s="6" t="n">
         <v>5362.73066</v>
@@ -3704,7 +3696,7 @@
     </row>
     <row r="157" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B157" s="6" t="n">
         <v>5324.68427</v>
@@ -3722,7 +3714,7 @@
     </row>
     <row r="158" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B158" s="6" t="n">
         <v>5323.68804</v>
@@ -3740,7 +3732,7 @@
     </row>
     <row r="159" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B159" s="6" t="n">
         <v>5308.71233</v>
@@ -3758,7 +3750,7 @@
     </row>
     <row r="160" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B160" s="6" t="n">
         <v>5307.70576</v>
@@ -3776,7 +3768,7 @@
     </row>
     <row r="161" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B161" s="6" t="n">
         <v>5307.70576</v>
@@ -3794,7 +3786,7 @@
     </row>
     <row r="162" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B162" s="6" t="n">
         <v>5303.83808</v>
@@ -3812,7 +3804,7 @@
     </row>
     <row r="163" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B163" s="6" t="n">
         <v>5293.73132</v>
@@ -3830,7 +3822,7 @@
     </row>
     <row r="164" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B164" s="6" t="n">
         <v>5291.7282</v>
@@ -3848,7 +3840,7 @@
     </row>
     <row r="165" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B165" s="6" t="n">
         <v>5288.64863</v>
@@ -3866,7 +3858,7 @@
     </row>
     <row r="166" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B166" s="6" t="n">
         <v>5252.63738</v>
@@ -3884,7 +3876,7 @@
     </row>
     <row r="167" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B167" s="6" t="n">
         <v>5244.6955</v>
@@ -3902,7 +3894,7 @@
     </row>
     <row r="168" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B168" s="6" t="n">
         <v>5240.72072</v>
@@ -3920,7 +3912,7 @@
     </row>
     <row r="169" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B169" s="6" t="n">
         <v>5237.68466</v>
@@ -3938,7 +3930,7 @@
     </row>
     <row r="170" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B170" s="6" t="n">
         <v>5236.67744</v>
@@ -3956,7 +3948,7 @@
     </row>
     <row r="171" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B171" s="6" t="n">
         <v>5236.67519</v>
@@ -3974,7 +3966,7 @@
     </row>
     <row r="172" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B172" s="6" t="n">
         <v>5231.80627</v>
@@ -3992,7 +3984,7 @@
     </row>
     <row r="173" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B173" s="6" t="n">
         <v>5230.77851</v>
@@ -4010,7 +4002,7 @@
     </row>
     <row r="174" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B174" s="6" t="n">
         <v>5223.69679</v>
@@ -4028,7 +4020,7 @@
     </row>
     <row r="175" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B175" s="6" t="n">
         <v>5221.6903</v>
@@ -4046,7 +4038,7 @@
     </row>
     <row r="176" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B176" s="6" t="n">
         <v>5220.68703</v>
@@ -4064,7 +4056,7 @@
     </row>
     <row r="177" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B177" s="6" t="n">
         <v>5216.60566</v>
@@ -4082,7 +4074,7 @@
     </row>
     <row r="178" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B178" s="6" t="n">
         <v>5204.20986</v>
@@ -4100,7 +4092,7 @@
     </row>
     <row r="179" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B179" s="6" t="n">
         <v>5182.63007</v>
@@ -4118,7 +4110,7 @@
     </row>
     <row r="180" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B180" s="6" t="n">
         <v>5181.6041</v>
@@ -4136,7 +4128,7 @@
     </row>
     <row r="181" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B181" s="6" t="n">
         <v>5172.6487</v>
@@ -4154,7 +4146,7 @@
     </row>
     <row r="182" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B182" s="6" t="n">
         <v>5168.18239</v>
@@ -4172,7 +4164,7 @@
     </row>
     <row r="183" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B183" s="6" t="n">
         <v>5165.64716</v>
@@ -4190,7 +4182,7 @@
     </row>
     <row r="184" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B184" s="6" t="n">
         <v>5160.75774</v>
@@ -4208,7 +4200,7 @@
     </row>
     <row r="185" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B185" s="6" t="n">
         <v>5153.66479</v>
@@ -4226,7 +4218,7 @@
     </row>
     <row r="186" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B186" s="6" t="n">
         <v>5150.65515</v>
@@ -4244,7 +4236,7 @@
     </row>
     <row r="187" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B187" s="6" t="n">
         <v>5146.57734</v>
@@ -4262,7 +4254,7 @@
     </row>
     <row r="188" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B188" s="6" t="n">
         <v>5145.57685</v>
@@ -4280,7 +4272,7 @@
     </row>
     <row r="189" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B189" s="6" t="n">
         <v>5111.58466</v>
@@ -4298,7 +4290,7 @@
     </row>
     <row r="190" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B190" s="6" t="n">
         <v>5110.59435</v>
@@ -4316,7 +4308,7 @@
     </row>
     <row r="191" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B191" s="6" t="n">
         <v>5110.56151</v>
@@ -4334,7 +4326,7 @@
     </row>
     <row r="192" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B192" s="6" t="n">
         <v>5094.60316</v>
@@ -4352,7 +4344,7 @@
     </row>
     <row r="193" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B193" s="6" t="n">
         <v>5089.72236</v>
@@ -4370,7 +4362,7 @@
     </row>
     <row r="194" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B194" s="6" t="n">
         <v>5088.72187</v>
@@ -4388,7 +4380,7 @@
     </row>
     <row r="195" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B195" s="6" t="n">
         <v>5080.61883</v>
@@ -4406,7 +4398,7 @@
     </row>
     <row r="196" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B196" s="6" t="n">
         <v>5078.61233</v>
@@ -4424,7 +4416,7 @@
     </row>
     <row r="197" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B197" s="6" t="n">
         <v>5078.58466</v>
@@ -4442,7 +4434,7 @@
     </row>
     <row r="198" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B198" s="6" t="n">
         <v>5043.53681</v>
@@ -4460,7 +4452,7 @@
     </row>
     <row r="199" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B199" s="6" t="n">
         <v>5040.57099</v>
@@ -4478,7 +4470,7 @@
     </row>
     <row r="200" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B200" s="6" t="n">
         <v>5039.58027</v>

</xml_diff>